<commit_message>
updated sample document for interpreter bulk updates
</commit_message>
<xml_diff>
--- a/public/assets/Mediators_Upload_Sample_Document.xlsx
+++ b/public/assets/Mediators_Upload_Sample_Document.xlsx
@@ -22,10 +22,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
-    <t xml:space="preserve">firstName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lastName</t>
+    <t xml:space="preserve">first_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">last_name</t>
   </si>
   <si>
     <t xml:space="preserve">email</t>
@@ -192,16 +192,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -397,7 +393,7 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -504,11 +500,11 @@
       <c r="O2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="P2" s="2" t="b">
+      <c r="P2" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="Q2" s="2" t="b">
+      <c r="Q2" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>

</xml_diff>